<commit_message>
add tutorial project to folder
</commit_message>
<xml_diff>
--- a/To Touch the Moon.xlsx
+++ b/To Touch the Moon.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joe Wahbeh\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joe Wahbeh\Desktop\ToTouchTheMoon.Solution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA08C8A9-C64B-4452-B92A-A8DD92900406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8627F47F-670B-4DDF-B6F0-3ADD7C92D7E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{082D898A-D4C4-4EC7-A241-265944D0234C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{082D898A-D4C4-4EC7-A241-265944D0234C}"/>
   </bookViews>
   <sheets>
     <sheet name="Links" sheetId="9" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="254">
   <si>
     <t>To Touch the Moon</t>
   </si>
@@ -732,6 +732,69 @@
   </si>
   <si>
     <t>fur</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>melee damage, main carrying capacity</t>
+  </si>
+  <si>
+    <t>luck</t>
+  </si>
+  <si>
+    <t>lots of minor things, helps crit chance evade traps,</t>
+  </si>
+  <si>
+    <t>Hp</t>
+  </si>
+  <si>
+    <t>Hit points</t>
+  </si>
+  <si>
+    <t>Mp</t>
+  </si>
+  <si>
+    <t>Mana points</t>
+  </si>
+  <si>
+    <t>Ep</t>
+  </si>
+  <si>
+    <t>Energy points</t>
+  </si>
+  <si>
+    <t>defence against lots of monster abilities, minor hp and mp</t>
+  </si>
+  <si>
+    <t>missile damage, minor increase in evasion</t>
+  </si>
+  <si>
+    <t>main hp increase, minor carrying capacity</t>
+  </si>
+  <si>
+    <t>shop discount</t>
+  </si>
+  <si>
+    <t>helps to learn magic, increases mp regen</t>
+  </si>
+  <si>
+    <t>increase Mp, protect against some special abilities</t>
+  </si>
+  <si>
+    <t>increase skill die, high wisdom can grants some minor luck</t>
+  </si>
+  <si>
+    <t>Reward: some of there old equipment</t>
+  </si>
+  <si>
+    <t>Clive is a Calvary / horse rider</t>
+  </si>
+  <si>
+    <t>Matilda is a Valkryie</t>
+  </si>
+  <si>
+    <t>It shall be engraved on your soul</t>
   </si>
 </sst>
 </file>
@@ -1124,10 +1187,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A675274B-B03F-4524-BB5C-559A52553DDE}">
-  <dimension ref="A1:Q49"/>
+  <dimension ref="A1:U49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3:U13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1136,130 +1199,186 @@
     <col min="5" max="5" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="U4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H5" t="s">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="L5" t="s">
         <v>117</v>
       </c>
-      <c r="J5" t="s">
+      <c r="N5" t="s">
         <v>123</v>
       </c>
-      <c r="L5" t="s">
+      <c r="P5" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
-      <c r="H6" t="s">
+      <c r="C6" t="s">
+        <v>234</v>
+      </c>
+      <c r="L6" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
-      <c r="H7" t="s">
+      <c r="C7" t="s">
+        <v>247</v>
+      </c>
+      <c r="L7" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
-      <c r="H8" t="s">
+      <c r="C8" t="s">
+        <v>249</v>
+      </c>
+      <c r="L8" t="s">
         <v>119</v>
       </c>
-      <c r="I8" t="s">
+      <c r="M8" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
-      <c r="H9" t="s">
+      <c r="C9" t="s">
+        <v>246</v>
+      </c>
+      <c r="L9" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
-      <c r="H11" t="s">
+      <c r="C11" t="s">
+        <v>245</v>
+      </c>
+      <c r="L11" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
-      <c r="H12" t="s">
+      <c r="C12" t="s">
+        <v>243</v>
+      </c>
+      <c r="L12" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>235</v>
+      </c>
+      <c r="C15" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I18" t="s">
+        <v>237</v>
+      </c>
+      <c r="J18" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I19" t="s">
+        <v>239</v>
+      </c>
+      <c r="J19" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I20" t="s">
+        <v>241</v>
+      </c>
+      <c r="J20" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>107</v>
       </c>
@@ -1490,8 +1609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0366ED29-AD01-4E85-8D44-F09409CBE602}">
   <dimension ref="A1:AA14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1549,6 +1668,9 @@
       <c r="L4" t="s">
         <v>203</v>
       </c>
+      <c r="T4" t="s">
+        <v>253</v>
+      </c>
       <c r="AA4" t="s">
         <v>55</v>
       </c>
@@ -1652,10 +1774,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20D1507C-D476-4BC6-914E-A05FCC418F72}">
-  <dimension ref="A2:X10"/>
+  <dimension ref="A2:X19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R12" sqref="R12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1754,6 +1876,86 @@
       </c>
       <c r="R10" t="s">
         <v>223</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="K13" t="s">
+        <v>233</v>
+      </c>
+      <c r="L13" t="s">
+        <v>233</v>
+      </c>
+      <c r="M13" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="J14" t="s">
+        <v>233</v>
+      </c>
+      <c r="K14" t="s">
+        <v>233</v>
+      </c>
+      <c r="M14" t="s">
+        <v>233</v>
+      </c>
+      <c r="N14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="I15" t="s">
+        <v>233</v>
+      </c>
+      <c r="J15" t="s">
+        <v>233</v>
+      </c>
+      <c r="N15" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="I16" t="s">
+        <v>233</v>
+      </c>
+      <c r="O16" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="17" spans="10:15" x14ac:dyDescent="0.25">
+      <c r="J17" t="s">
+        <v>233</v>
+      </c>
+      <c r="N17" t="s">
+        <v>233</v>
+      </c>
+      <c r="O17" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="18" spans="10:15" x14ac:dyDescent="0.25">
+      <c r="J18" t="s">
+        <v>233</v>
+      </c>
+      <c r="K18" t="s">
+        <v>233</v>
+      </c>
+      <c r="M18" t="s">
+        <v>233</v>
+      </c>
+      <c r="N18" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="19" spans="10:15" x14ac:dyDescent="0.25">
+      <c r="K19" t="s">
+        <v>233</v>
+      </c>
+      <c r="L19" t="s">
+        <v>233</v>
+      </c>
+      <c r="M19" t="s">
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -1766,10 +1968,13 @@
   <dimension ref="A3:U29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="19" max="19" width="11.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -2053,7 +2258,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2210,46 +2415,57 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B205239A-D48A-4E40-A55C-B90DA2BD8838}">
-  <dimension ref="A3:A11"/>
+  <dimension ref="A3:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>251</v>
+      </c>
+      <c r="H3" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>194</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add aactual project to solution
</commit_message>
<xml_diff>
--- a/To Touch the Moon.xlsx
+++ b/To Touch the Moon.xlsx
@@ -8,20 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joe Wahbeh\Desktop\ToTouchTheMoon.Solution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24B9C98D-F423-48A2-A841-ACFEECA0AFF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51592DF7-A9DD-4822-A58E-7CA210B72BE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-60" windowWidth="29040" windowHeight="15840" xr2:uid="{082D898A-D4C4-4EC7-A241-265944D0234C}"/>
+    <workbookView xWindow="28680" yWindow="-60" windowWidth="29040" windowHeight="15840" tabRatio="731" firstSheet="1" activeTab="11" xr2:uid="{082D898A-D4C4-4EC7-A241-265944D0234C}"/>
   </bookViews>
   <sheets>
     <sheet name="Links" sheetId="9" r:id="rId1"/>
     <sheet name="Character Creation" sheetId="1" r:id="rId2"/>
     <sheet name="Spell List" sheetId="8" r:id="rId3"/>
     <sheet name="Names" sheetId="2" r:id="rId4"/>
-    <sheet name="procedurally generated" sheetId="5" r:id="rId5"/>
-    <sheet name="Lore" sheetId="3" r:id="rId6"/>
-    <sheet name="Controls" sheetId="4" r:id="rId7"/>
-    <sheet name="Game Mechanic Ideas" sheetId="6" r:id="rId8"/>
-    <sheet name="Quests" sheetId="7" r:id="rId9"/>
+    <sheet name="Sheet1" sheetId="11" r:id="rId5"/>
+    <sheet name="procedurally generated" sheetId="5" r:id="rId6"/>
+    <sheet name="Lore" sheetId="3" r:id="rId7"/>
+    <sheet name="Controls" sheetId="4" r:id="rId8"/>
+    <sheet name="Game Mechanic Ideas" sheetId="6" r:id="rId9"/>
+    <sheet name="Quests" sheetId="7" r:id="rId10"/>
+    <sheet name="Monsters" sheetId="10" r:id="rId11"/>
+    <sheet name="Corruptions" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="316">
   <si>
     <t>To Touch the Moon</t>
   </si>
@@ -804,6 +807,183 @@
   </si>
   <si>
     <t>place to get fonts</t>
+  </si>
+  <si>
+    <t>https://www.text-image.com/convert/ascii.html</t>
+  </si>
+  <si>
+    <t>https://github.com/Thraka/SadConsole</t>
+  </si>
+  <si>
+    <t>image to ascii converter</t>
+  </si>
+  <si>
+    <t>SadConsole github</t>
+  </si>
+  <si>
+    <t>https://markjames.dev/2020-05-21-making-a-roguelike-in-c-with-gorogue-sadconsole-part-one/</t>
+  </si>
+  <si>
+    <t>Sad console tutorial</t>
+  </si>
+  <si>
+    <t>https://code2d.wordpress.com/sadconsole-tutorials/</t>
+  </si>
+  <si>
+    <t>Sad  Console tutorial</t>
+  </si>
+  <si>
+    <t>https://share.text-image.com/67e70ca32cf421d6</t>
+  </si>
+  <si>
+    <t>Animals</t>
+  </si>
+  <si>
+    <t>Constructs</t>
+  </si>
+  <si>
+    <t>Undead</t>
+  </si>
+  <si>
+    <t>Demons</t>
+  </si>
+  <si>
+    <t>Humanoid</t>
+  </si>
+  <si>
+    <t>Giants</t>
+  </si>
+  <si>
+    <t>Dragons</t>
+  </si>
+  <si>
+    <t>Machines made from past or future civilizations</t>
+  </si>
+  <si>
+    <t>to angry to die</t>
+  </si>
+  <si>
+    <t>Angels</t>
+  </si>
+  <si>
+    <t>Servants of Luna - Beings of Chaos</t>
+  </si>
+  <si>
+    <t>Servants of Sol - Beings of Order</t>
+  </si>
+  <si>
+    <t>have human like traits</t>
+  </si>
+  <si>
+    <t>sub category of humanoid - tall beings</t>
+  </si>
+  <si>
+    <t>Strong monsters</t>
+  </si>
+  <si>
+    <t>Almost always neutral</t>
+  </si>
+  <si>
+    <t>Monster Prefix</t>
+  </si>
+  <si>
+    <t>Monster Suffix</t>
+  </si>
+  <si>
+    <t>Raging</t>
+  </si>
+  <si>
+    <t>will spawn friendly for neutral and lawful, 50/50 for chaos. Killing them will lose favor with that god unless chaotic and being chaotic. Luna finds it amusing when her minions fight each other.</t>
+  </si>
+  <si>
+    <t>Serene</t>
+  </si>
+  <si>
+    <t>Generated peaceful regarless of alignment</t>
+  </si>
+  <si>
+    <t>Generated Hostile regardless of alignment - unable to be calmed down</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +5 Levels of expereince to monster</t>
+  </si>
+  <si>
+    <t>of  *element type*</t>
+  </si>
+  <si>
+    <t>extra 10% damage done is added to attack. I.E if monster roles 50 damage before calculations they will do +5 *elemental* damage added to final attack.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>http://sadconsole.com/v9/api/</t>
+  </si>
+  <si>
+    <t>Link to SadConsole Documentation</t>
+  </si>
+  <si>
+    <t>Lion</t>
+  </si>
+  <si>
+    <t>Bear</t>
+  </si>
+  <si>
+    <t>Arctic Bear</t>
+  </si>
+  <si>
+    <t>Iron Golem</t>
+  </si>
+  <si>
+    <t>Steel Golem</t>
+  </si>
+  <si>
+    <t>Mithril Golem</t>
+  </si>
+  <si>
+    <t>Zombie</t>
+  </si>
+  <si>
+    <t>ghost</t>
+  </si>
+  <si>
+    <t>vampire</t>
+  </si>
+  <si>
+    <t>Dullahan</t>
+  </si>
+  <si>
+    <t>Blade of Pandemonium</t>
+  </si>
+  <si>
+    <t>Roxy's Holy Relic</t>
+  </si>
+  <si>
+    <t>Aylas Holy Scarf</t>
+  </si>
+  <si>
+    <t>Scepter of the Heavenly King</t>
+  </si>
+  <si>
+    <t>Of Two Minds</t>
+  </si>
+  <si>
+    <t>gain an extra turn of movement that is randomly used</t>
+  </si>
+  <si>
+    <t>You feel as if your mind was split in two</t>
+  </si>
+  <si>
+    <t>Of 2 Minds</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -2 int, -1 learning</t>
+  </si>
+  <si>
+    <t>You feel as if your mind has abosrbed another entitiy</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +2 int, + 1 learning</t>
   </si>
 </sst>
 </file>
@@ -1176,28 +1356,360 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{693DF346-5D15-4F5D-9B48-9E9CDA19D07C}">
-  <dimension ref="A2:H5"/>
+  <dimension ref="A2:O17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>195</v>
       </c>
-      <c r="H2" t="s">
+      <c r="L2" t="s">
         <v>255</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>254</v>
+      </c>
+      <c r="L5" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>257</v>
+      </c>
+      <c r="L6" t="s">
+        <v>259</v>
+      </c>
+      <c r="O6" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>258</v>
+      </c>
+      <c r="L9" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>261</v>
+      </c>
+      <c r="L12" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>263</v>
+      </c>
+      <c r="L14" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>293</v>
+      </c>
+      <c r="L17" t="s">
+        <v>294</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B205239A-D48A-4E40-A55C-B90DA2BD8838}">
+  <dimension ref="A3:H13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E3" t="s">
+        <v>251</v>
+      </c>
+      <c r="H3" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>254</v>
-      </c>
-      <c r="H5" t="s">
-        <v>256</v>
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>194</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83AA777F-5A06-40E5-B322-E8F11D33EFDB}">
+  <dimension ref="A1:S26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>282</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>284</v>
+      </c>
+      <c r="C13" t="s">
+        <v>288</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>146</v>
+      </c>
+      <c r="S13" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>286</v>
+      </c>
+      <c r="C14" t="s">
+        <v>287</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>290</v>
+      </c>
+      <c r="S14" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>158</v>
+      </c>
+      <c r="C15" t="s">
+        <v>289</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>266</v>
+      </c>
+      <c r="C21" t="s">
+        <v>267</v>
+      </c>
+      <c r="E21" t="s">
+        <v>268</v>
+      </c>
+      <c r="G21" t="s">
+        <v>269</v>
+      </c>
+      <c r="I21" t="s">
+        <v>275</v>
+      </c>
+      <c r="K21" t="s">
+        <v>270</v>
+      </c>
+      <c r="M21" t="s">
+        <v>271</v>
+      </c>
+      <c r="O21" t="s">
+        <v>272</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>295</v>
+      </c>
+      <c r="C23" t="s">
+        <v>298</v>
+      </c>
+      <c r="E23" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>296</v>
+      </c>
+      <c r="C24" t="s">
+        <v>299</v>
+      </c>
+      <c r="E24" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>297</v>
+      </c>
+      <c r="C25" t="s">
+        <v>300</v>
+      </c>
+      <c r="E25" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>304</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9817146-B7F1-4C77-98EA-19ABF1317FD6}">
+  <dimension ref="A1:K7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D1" t="s">
+        <v>150</v>
+      </c>
+      <c r="K1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>309</v>
+      </c>
+      <c r="D3" t="s">
+        <v>310</v>
+      </c>
+      <c r="K3" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>312</v>
+      </c>
+      <c r="D6" t="s">
+        <v>310</v>
+      </c>
+      <c r="K6" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>315</v>
       </c>
     </row>
   </sheetData>
@@ -1209,8 +1721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A675274B-B03F-4524-BB5C-559A52553DDE}">
   <dimension ref="A1:U49"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3:U13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1627,10 +2139,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0366ED29-AD01-4E85-8D44-F09409CBE602}">
-  <dimension ref="A1:AA14"/>
+  <dimension ref="A1:AA19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T4" sqref="T4"/>
+      <selection activeCell="Q39" sqref="Q39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1787,12 +2299,44 @@
         <v>216</v>
       </c>
     </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="I16" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="17" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I17" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="18" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I18" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="19" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I19" t="s">
+        <v>307</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB6F68B4-09EC-4065-B5C0-D4F7B5E690E0}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20D1507C-D476-4BC6-914E-A05FCC418F72}">
   <dimension ref="A2:X19"/>
   <sheetViews>
@@ -1983,7 +2527,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52B3DB97-1DD0-49AA-A2A9-5C5AF5717736}">
   <dimension ref="A3:U29"/>
   <sheetViews>
@@ -2273,7 +2817,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E49DEAA8-706B-448E-82BE-2C963842E1B1}">
   <dimension ref="A1:E14"/>
   <sheetViews>
@@ -2408,7 +2952,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{416AE8D8-06A2-47F0-B834-06EC48ADCB4C}">
   <dimension ref="A4:A6"/>
   <sheetViews>
@@ -2431,66 +2975,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B205239A-D48A-4E40-A55C-B90DA2BD8838}">
-  <dimension ref="A3:H13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="E3" t="s">
-        <v>251</v>
-      </c>
-      <c r="H3" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>194</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>